<commit_message>
add other racial groups into national poverty table
</commit_message>
<xml_diff>
--- a/raw_data/national/national_poverty.xlsx
+++ b/raw_data/national/national_poverty.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/temp/AAPIData_quickstats_master/raw_data/national/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/temp/Dropbox/AAPIData HQ/AAPI QuickStats/redesign/national level/ready4github/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14320"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="9">
   <si>
     <t>geodisplaylabel</t>
   </si>
@@ -365,7 +365,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H68"/>
+  <dimension ref="A1:H72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -430,22 +430,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C3">
-        <v>15922215</v>
+        <v>38228744</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>2000884</v>
+        <v>10321254</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>13921331</v>
+        <v>27907492</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -456,22 +456,22 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>3257958</v>
+        <v>2481414</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>253140</v>
+        <v>702127</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>3004818</v>
+        <v>1779287</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -482,22 +482,22 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5">
-        <v>151964</v>
+        <v>15922215</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>37430</v>
+        <v>2000884</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>114534</v>
+        <v>13921331</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -508,22 +508,22 @@
         <v>1</v>
       </c>
       <c r="B6">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6">
-        <v>259769</v>
+        <v>3257958</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>51121</v>
+        <v>253140</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>208648</v>
+        <v>3004818</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -534,22 +534,22 @@
         <v>1</v>
       </c>
       <c r="B7">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7">
-        <v>3741069</v>
+        <v>151964</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>579743</v>
+        <v>37430</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>3161326</v>
+        <v>114534</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -560,22 +560,22 @@
         <v>1</v>
       </c>
       <c r="B8">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C8">
-        <v>3587711</v>
+        <v>259769</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
       <c r="E8">
-        <v>560097</v>
+        <v>51121</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8">
-        <v>3027614</v>
+        <v>208648</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -586,22 +586,22 @@
         <v>1</v>
       </c>
       <c r="B9">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9">
-        <v>143801</v>
+        <v>3741069</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>18575</v>
+        <v>579743</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
-        <v>125226</v>
+        <v>3161326</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -612,22 +612,22 @@
         <v>1</v>
       </c>
       <c r="B10">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C10">
-        <v>2686027</v>
+        <v>3587711</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10">
-        <v>181911</v>
+        <v>560097</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10">
-        <v>2504116</v>
+        <v>3027614</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -638,22 +638,22 @@
         <v>1</v>
       </c>
       <c r="B11">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C11">
-        <v>262953</v>
+        <v>143801</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11">
-        <v>68974</v>
+        <v>18575</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
-        <v>193979</v>
+        <v>125226</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -664,22 +664,22 @@
         <v>1</v>
       </c>
       <c r="B12">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C12">
-        <v>69904</v>
+        <v>2686027</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12">
-        <v>10571</v>
+        <v>181911</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
       <c r="G12">
-        <v>59333</v>
+        <v>2504116</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -690,22 +690,22 @@
         <v>1</v>
       </c>
       <c r="B13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C13">
-        <v>763887</v>
+        <v>262953</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13">
-        <v>61975</v>
+        <v>68974</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13">
-        <v>701912</v>
+        <v>193979</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -716,22 +716,22 @@
         <v>1</v>
       </c>
       <c r="B14">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C14">
-        <v>1415892</v>
+        <v>69904</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14">
-        <v>203490</v>
+        <v>10571</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
       <c r="G14">
-        <v>1212402</v>
+        <v>59333</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -742,22 +742,22 @@
         <v>1</v>
       </c>
       <c r="B15">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C15">
-        <v>204904</v>
+        <v>763887</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15">
-        <v>34237</v>
+        <v>61975</v>
       </c>
       <c r="F15">
         <v>0</v>
       </c>
       <c r="G15">
-        <v>170667</v>
+        <v>701912</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -768,22 +768,22 @@
         <v>1</v>
       </c>
       <c r="B16">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C16">
-        <v>17898</v>
+        <v>1415892</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16">
-        <v>4497</v>
+        <v>203490</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="G16">
-        <v>13401</v>
+        <v>1212402</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -794,22 +794,22 @@
         <v>1</v>
       </c>
       <c r="B17">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C17">
-        <v>410038</v>
+        <v>204904</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17">
-        <v>69068</v>
+        <v>34237</v>
       </c>
       <c r="F17">
         <v>0</v>
       </c>
       <c r="G17">
-        <v>340970</v>
+        <v>170667</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -820,22 +820,22 @@
         <v>1</v>
       </c>
       <c r="B18">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C18">
-        <v>44958</v>
+        <v>17898</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18">
-        <v>5080</v>
+        <v>4497</v>
       </c>
       <c r="F18">
         <v>0</v>
       </c>
       <c r="G18">
-        <v>39878</v>
+        <v>13401</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -846,22 +846,22 @@
         <v>1</v>
       </c>
       <c r="B19">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C19">
-        <v>185238</v>
+        <v>410038</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>30896</v>
+        <v>69068</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
       <c r="G19">
-        <v>154342</v>
+        <v>340970</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -872,22 +872,22 @@
         <v>1</v>
       </c>
       <c r="B20">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C20">
-        <v>1684950</v>
+        <v>44958</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20">
-        <v>257658</v>
+        <v>5080</v>
       </c>
       <c r="F20">
         <v>0</v>
       </c>
       <c r="G20">
-        <v>1427292</v>
+        <v>39878</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -898,22 +898,22 @@
         <v>1</v>
       </c>
       <c r="B21">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C21">
-        <v>18781840</v>
+        <v>185238</v>
       </c>
       <c r="D21">
         <v>0</v>
       </c>
       <c r="E21">
-        <v>2359834</v>
+        <v>30896</v>
       </c>
       <c r="F21">
         <v>0</v>
       </c>
       <c r="G21">
-        <v>16422007</v>
+        <v>154342</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -924,22 +924,22 @@
         <v>1</v>
       </c>
       <c r="B22">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C22">
-        <v>3538420</v>
+        <v>1684950</v>
       </c>
       <c r="D22">
         <v>0</v>
       </c>
       <c r="E22">
-        <v>287457</v>
+        <v>257658</v>
       </c>
       <c r="F22">
         <v>0</v>
       </c>
       <c r="G22">
-        <v>3250963</v>
+        <v>1427292</v>
       </c>
       <c r="H22">
         <v>0</v>
@@ -950,22 +950,22 @@
         <v>1</v>
       </c>
       <c r="B23">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C23">
-        <v>163362</v>
+        <v>18781840</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23">
-        <v>39732</v>
+        <v>2359834</v>
       </c>
       <c r="F23">
         <v>0</v>
       </c>
       <c r="G23">
-        <v>123630</v>
+        <v>16422007</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -976,22 +976,22 @@
         <v>1</v>
       </c>
       <c r="B24">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C24">
-        <v>311980</v>
+        <v>3538420</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24">
-        <v>61846</v>
+        <v>287457</v>
       </c>
       <c r="F24">
         <v>0</v>
       </c>
       <c r="G24">
-        <v>250134</v>
+        <v>3250963</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -1002,22 +1002,22 @@
         <v>1</v>
       </c>
       <c r="B25">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C25">
-        <v>4466002</v>
+        <v>163362</v>
       </c>
       <c r="D25">
         <v>0</v>
       </c>
       <c r="E25">
-        <v>651799</v>
+        <v>39732</v>
       </c>
       <c r="F25">
         <v>0</v>
       </c>
       <c r="G25">
-        <v>3814203</v>
+        <v>123630</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -1028,22 +1028,22 @@
         <v>1</v>
       </c>
       <c r="B26">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C26">
-        <v>4301605</v>
+        <v>311980</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
       <c r="E26">
-        <v>631507</v>
+        <v>61846</v>
       </c>
       <c r="F26">
         <v>0</v>
       </c>
       <c r="G26">
-        <v>3670098</v>
+        <v>250134</v>
       </c>
       <c r="H26">
         <v>0</v>
@@ -1054,22 +1054,22 @@
         <v>1</v>
       </c>
       <c r="B27">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C27">
-        <v>175413</v>
+        <v>4466002</v>
       </c>
       <c r="D27">
         <v>0</v>
       </c>
       <c r="E27">
-        <v>21466</v>
+        <v>651799</v>
       </c>
       <c r="F27">
         <v>0</v>
       </c>
       <c r="G27">
-        <v>153947</v>
+        <v>3814203</v>
       </c>
       <c r="H27">
         <v>0</v>
@@ -1080,22 +1080,22 @@
         <v>1</v>
       </c>
       <c r="B28">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C28">
-        <v>3653059</v>
+        <v>4301605</v>
       </c>
       <c r="D28">
         <v>0</v>
       </c>
       <c r="E28">
-        <v>287471</v>
+        <v>631507</v>
       </c>
       <c r="F28">
         <v>0</v>
       </c>
       <c r="G28">
-        <v>3365588</v>
+        <v>3670098</v>
       </c>
       <c r="H28">
         <v>0</v>
@@ -1106,22 +1106,22 @@
         <v>1</v>
       </c>
       <c r="B29">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C29">
-        <v>276038</v>
+        <v>175413</v>
       </c>
       <c r="D29">
         <v>0</v>
       </c>
       <c r="E29">
-        <v>72119</v>
+        <v>21466</v>
       </c>
       <c r="F29">
         <v>0</v>
       </c>
       <c r="G29">
-        <v>203919</v>
+        <v>153947</v>
       </c>
       <c r="H29">
         <v>0</v>
@@ -1132,22 +1132,22 @@
         <v>1</v>
       </c>
       <c r="B30">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C30">
-        <v>105935</v>
+        <v>3653059</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
       <c r="E30">
-        <v>14571</v>
+        <v>287471</v>
       </c>
       <c r="F30">
         <v>0</v>
       </c>
       <c r="G30">
-        <v>91364</v>
+        <v>3365588</v>
       </c>
       <c r="H30">
         <v>0</v>
@@ -1158,22 +1158,22 @@
         <v>1</v>
       </c>
       <c r="B31">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C31">
-        <v>1356610</v>
+        <v>276038</v>
       </c>
       <c r="D31">
         <v>0</v>
       </c>
       <c r="E31">
-        <v>119892</v>
+        <v>72119</v>
       </c>
       <c r="F31">
         <v>0</v>
       </c>
       <c r="G31">
-        <v>1236718</v>
+        <v>203919</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -1184,22 +1184,22 @@
         <v>1</v>
       </c>
       <c r="B32">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C32">
-        <v>1739922</v>
+        <v>105935</v>
       </c>
       <c r="D32">
         <v>0</v>
       </c>
       <c r="E32">
-        <v>237275</v>
+        <v>14571</v>
       </c>
       <c r="F32">
         <v>0</v>
       </c>
       <c r="G32">
-        <v>1502647</v>
+        <v>91364</v>
       </c>
       <c r="H32">
         <v>0</v>
@@ -1210,22 +1210,22 @@
         <v>1</v>
       </c>
       <c r="B33">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C33">
-        <v>252011</v>
+        <v>1356610</v>
       </c>
       <c r="D33">
         <v>0</v>
       </c>
       <c r="E33">
-        <v>41909</v>
+        <v>119892</v>
       </c>
       <c r="F33">
         <v>0</v>
       </c>
       <c r="G33">
-        <v>210102</v>
+        <v>1236718</v>
       </c>
       <c r="H33">
         <v>0</v>
@@ -1236,22 +1236,22 @@
         <v>1</v>
       </c>
       <c r="B34">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C34">
-        <v>27287</v>
+        <v>1739922</v>
       </c>
       <c r="D34">
         <v>0</v>
       </c>
       <c r="E34">
-        <v>5616</v>
+        <v>237275</v>
       </c>
       <c r="F34">
         <v>0</v>
       </c>
       <c r="G34">
-        <v>21671</v>
+        <v>1502647</v>
       </c>
       <c r="H34">
         <v>0</v>
@@ -1262,22 +1262,22 @@
         <v>1</v>
       </c>
       <c r="B35">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C35">
-        <v>449360</v>
+        <v>252011</v>
       </c>
       <c r="D35">
         <v>0</v>
       </c>
       <c r="E35">
-        <v>74373</v>
+        <v>41909</v>
       </c>
       <c r="F35">
         <v>0</v>
       </c>
       <c r="G35">
-        <v>374987</v>
+        <v>210102</v>
       </c>
       <c r="H35">
         <v>0</v>
@@ -1288,22 +1288,22 @@
         <v>1</v>
       </c>
       <c r="B36">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C36">
-        <v>50957</v>
+        <v>27287</v>
       </c>
       <c r="D36">
         <v>0</v>
       </c>
       <c r="E36">
-        <v>5530</v>
+        <v>5616</v>
       </c>
       <c r="F36">
         <v>0</v>
       </c>
       <c r="G36">
-        <v>45427</v>
+        <v>21671</v>
       </c>
       <c r="H36">
         <v>0</v>
@@ -1314,22 +1314,22 @@
         <v>1</v>
       </c>
       <c r="B37">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C37">
-        <v>272682</v>
+        <v>449360</v>
       </c>
       <c r="D37">
         <v>0</v>
       </c>
       <c r="E37">
-        <v>42019</v>
+        <v>74373</v>
       </c>
       <c r="F37">
         <v>0</v>
       </c>
       <c r="G37">
-        <v>230663</v>
+        <v>374987</v>
       </c>
       <c r="H37">
         <v>0</v>
@@ -1340,22 +1340,22 @@
         <v>1</v>
       </c>
       <c r="B38">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C38">
-        <v>1897424</v>
+        <v>50957</v>
       </c>
       <c r="D38">
         <v>0</v>
       </c>
       <c r="E38">
-        <v>283890</v>
+        <v>5530</v>
       </c>
       <c r="F38">
         <v>0</v>
       </c>
       <c r="G38">
-        <v>1613534</v>
+        <v>45427</v>
       </c>
       <c r="H38">
         <v>0</v>
@@ -1366,22 +1366,22 @@
         <v>1</v>
       </c>
       <c r="B39">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C39">
-        <v>530274</v>
+        <v>272682</v>
       </c>
       <c r="D39">
         <v>0</v>
       </c>
       <c r="E39">
-        <v>111137</v>
+        <v>42019</v>
       </c>
       <c r="F39">
         <v>0</v>
       </c>
       <c r="G39">
-        <v>419137</v>
+        <v>230663</v>
       </c>
       <c r="H39">
         <v>0</v>
@@ -1392,22 +1392,22 @@
         <v>1</v>
       </c>
       <c r="B40">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C40">
-        <v>333655</v>
+        <v>1897424</v>
       </c>
       <c r="D40">
         <v>0</v>
       </c>
       <c r="E40">
-        <v>67292</v>
+        <v>283890</v>
       </c>
       <c r="F40">
         <v>0</v>
       </c>
       <c r="G40">
-        <v>266363</v>
+        <v>1613534</v>
       </c>
       <c r="H40">
         <v>0</v>
@@ -1418,22 +1418,22 @@
         <v>1</v>
       </c>
       <c r="B41">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C41">
-        <v>168159</v>
+        <v>530274</v>
       </c>
       <c r="D41">
         <v>0</v>
       </c>
       <c r="E41">
-        <v>32281</v>
+        <v>111137</v>
       </c>
       <c r="F41">
         <v>0</v>
       </c>
       <c r="G41">
-        <v>135878</v>
+        <v>419137</v>
       </c>
       <c r="H41">
         <v>0</v>
@@ -1444,22 +1444,22 @@
         <v>1</v>
       </c>
       <c r="B42">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C42">
-        <v>106253</v>
+        <v>333655</v>
       </c>
       <c r="D42">
         <v>0</v>
       </c>
       <c r="E42">
-        <v>22208</v>
+        <v>67292</v>
       </c>
       <c r="F42">
         <v>0</v>
       </c>
       <c r="G42">
-        <v>84045</v>
+        <v>266363</v>
       </c>
       <c r="H42">
         <v>0</v>
@@ -1470,22 +1470,22 @@
         <v>1</v>
       </c>
       <c r="B43">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C43">
-        <v>44732</v>
+        <v>168159</v>
       </c>
       <c r="D43">
         <v>0</v>
       </c>
       <c r="E43">
-        <v>9659</v>
+        <v>32281</v>
       </c>
       <c r="F43">
         <v>0</v>
       </c>
       <c r="G43">
-        <v>35073</v>
+        <v>135878</v>
       </c>
       <c r="H43">
         <v>0</v>
@@ -1496,22 +1496,22 @@
         <v>1</v>
       </c>
       <c r="B44">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C44">
-        <v>134969</v>
+        <v>106253</v>
       </c>
       <c r="D44">
         <v>0</v>
       </c>
       <c r="E44">
-        <v>34558</v>
+        <v>22208</v>
       </c>
       <c r="F44">
         <v>0</v>
       </c>
       <c r="G44">
-        <v>100411</v>
+        <v>84045</v>
       </c>
       <c r="H44">
         <v>0</v>
@@ -1522,22 +1522,22 @@
         <v>1</v>
       </c>
       <c r="B45">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C45">
-        <v>70945</v>
+        <v>44732</v>
       </c>
       <c r="D45">
         <v>0</v>
       </c>
       <c r="E45">
-        <v>10348</v>
+        <v>9659</v>
       </c>
       <c r="F45">
         <v>0</v>
       </c>
       <c r="G45">
-        <v>60597</v>
+        <v>35073</v>
       </c>
       <c r="H45">
         <v>0</v>
@@ -1548,22 +1548,22 @@
         <v>1</v>
       </c>
       <c r="B46">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C46">
-        <v>33581</v>
+        <v>134969</v>
       </c>
       <c r="D46">
         <v>0</v>
       </c>
       <c r="E46">
-        <v>3370</v>
+        <v>34558</v>
       </c>
       <c r="F46">
         <v>0</v>
       </c>
       <c r="G46">
-        <v>30211</v>
+        <v>100411</v>
       </c>
       <c r="H46">
         <v>0</v>
@@ -1574,22 +1574,22 @@
         <v>1</v>
       </c>
       <c r="B47">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C47">
-        <v>32900</v>
+        <v>70945</v>
       </c>
       <c r="D47">
         <v>0</v>
       </c>
       <c r="E47">
-        <v>3094</v>
+        <v>10348</v>
       </c>
       <c r="F47">
         <v>0</v>
       </c>
       <c r="G47">
-        <v>29806</v>
+        <v>60597</v>
       </c>
       <c r="H47">
         <v>0</v>
@@ -1600,22 +1600,22 @@
         <v>1</v>
       </c>
       <c r="B48">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C48">
-        <v>1223745</v>
+        <v>33581</v>
       </c>
       <c r="D48">
         <v>0</v>
       </c>
       <c r="E48">
-        <v>224583</v>
+        <v>3370</v>
       </c>
       <c r="F48">
         <v>0</v>
       </c>
       <c r="G48">
-        <v>999162</v>
+        <v>30211</v>
       </c>
       <c r="H48">
         <v>0</v>
@@ -1626,22 +1626,22 @@
         <v>1</v>
       </c>
       <c r="B49">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C49">
-        <v>761222</v>
+        <v>32900</v>
       </c>
       <c r="D49">
         <v>0</v>
       </c>
       <c r="E49">
-        <v>134067</v>
+        <v>3094</v>
       </c>
       <c r="F49">
         <v>0</v>
       </c>
       <c r="G49">
-        <v>627155</v>
+        <v>29806</v>
       </c>
       <c r="H49">
         <v>0</v>
@@ -1652,22 +1652,22 @@
         <v>1</v>
       </c>
       <c r="B50">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C50">
-        <v>534135</v>
+        <v>1223745</v>
       </c>
       <c r="D50">
         <v>0</v>
       </c>
       <c r="E50">
-        <v>88347</v>
+        <v>224583</v>
       </c>
       <c r="F50">
         <v>0</v>
       </c>
       <c r="G50">
-        <v>445788</v>
+        <v>999162</v>
       </c>
       <c r="H50">
         <v>0</v>
@@ -1678,22 +1678,22 @@
         <v>1</v>
       </c>
       <c r="B51">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C51">
-        <v>177571</v>
+        <v>761222</v>
       </c>
       <c r="D51">
         <v>0</v>
       </c>
       <c r="E51">
-        <v>36106</v>
+        <v>134067</v>
       </c>
       <c r="F51">
         <v>0</v>
       </c>
       <c r="G51">
-        <v>141465</v>
+        <v>627155</v>
       </c>
       <c r="H51">
         <v>0</v>
@@ -1704,22 +1704,22 @@
         <v>1</v>
       </c>
       <c r="B52">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C52">
-        <v>61258</v>
+        <v>534135</v>
       </c>
       <c r="D52">
         <v>0</v>
       </c>
       <c r="E52">
-        <v>13568</v>
+        <v>88347</v>
       </c>
       <c r="F52">
         <v>0</v>
       </c>
       <c r="G52">
-        <v>47690</v>
+        <v>445788</v>
       </c>
       <c r="H52">
         <v>0</v>
@@ -1730,22 +1730,22 @@
         <v>1</v>
       </c>
       <c r="B53">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C53">
-        <v>202135</v>
+        <v>177571</v>
       </c>
       <c r="D53">
         <v>0</v>
       </c>
       <c r="E53">
-        <v>46235</v>
+        <v>36106</v>
       </c>
       <c r="F53">
         <v>0</v>
       </c>
       <c r="G53">
-        <v>155900</v>
+        <v>141465</v>
       </c>
       <c r="H53">
         <v>0</v>
@@ -1756,22 +1756,22 @@
         <v>1</v>
       </c>
       <c r="B54">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C54">
-        <v>127022</v>
+        <v>61258</v>
       </c>
       <c r="D54">
         <v>0</v>
       </c>
       <c r="E54">
-        <v>18552</v>
+        <v>13568</v>
       </c>
       <c r="F54">
         <v>0</v>
       </c>
       <c r="G54">
-        <v>108470</v>
+        <v>47690</v>
       </c>
       <c r="H54">
         <v>0</v>
@@ -1782,22 +1782,22 @@
         <v>1</v>
       </c>
       <c r="B55">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C55">
-        <v>42151</v>
+        <v>202135</v>
       </c>
       <c r="D55">
         <v>0</v>
       </c>
       <c r="E55">
-        <v>4783</v>
+        <v>46235</v>
       </c>
       <c r="F55">
         <v>0</v>
       </c>
       <c r="G55">
-        <v>37368</v>
+        <v>155900</v>
       </c>
       <c r="H55">
         <v>0</v>
@@ -1808,22 +1808,22 @@
         <v>1</v>
       </c>
       <c r="B56">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C56">
-        <v>41181</v>
+        <v>127022</v>
       </c>
       <c r="D56">
         <v>0</v>
       </c>
       <c r="E56">
-        <v>4467</v>
+        <v>18552</v>
       </c>
       <c r="F56">
         <v>0</v>
       </c>
       <c r="G56">
-        <v>36714</v>
+        <v>108470</v>
       </c>
       <c r="H56">
         <v>0</v>
@@ -1834,22 +1834,22 @@
         <v>1</v>
       </c>
       <c r="B57">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C57">
-        <v>21371</v>
+        <v>42151</v>
       </c>
       <c r="D57">
         <v>0</v>
       </c>
       <c r="E57">
-        <v>7217</v>
+        <v>4783</v>
       </c>
       <c r="F57">
         <v>0</v>
       </c>
       <c r="G57">
-        <v>14154</v>
+        <v>37368</v>
       </c>
       <c r="H57">
         <v>0</v>
@@ -1860,22 +1860,22 @@
         <v>1</v>
       </c>
       <c r="B58">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C58">
-        <v>125506</v>
+        <v>41181</v>
       </c>
       <c r="D58">
         <v>0</v>
       </c>
       <c r="E58">
-        <v>49421</v>
+        <v>4467</v>
       </c>
       <c r="F58">
         <v>0</v>
       </c>
       <c r="G58">
-        <v>76085</v>
+        <v>36714</v>
       </c>
       <c r="H58">
         <v>0</v>
@@ -1886,22 +1886,22 @@
         <v>1</v>
       </c>
       <c r="B59">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C59">
-        <v>15465</v>
+        <v>21371</v>
       </c>
       <c r="D59">
         <v>0</v>
       </c>
       <c r="E59">
-        <v>4257</v>
+        <v>7217</v>
       </c>
       <c r="F59">
         <v>0</v>
       </c>
       <c r="G59">
-        <v>11208</v>
+        <v>14154</v>
       </c>
       <c r="H59">
         <v>0</v>
@@ -1912,22 +1912,22 @@
         <v>1</v>
       </c>
       <c r="B60">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C60">
-        <v>102132</v>
+        <v>125506</v>
       </c>
       <c r="D60">
         <v>0</v>
       </c>
       <c r="E60">
-        <v>26817</v>
+        <v>49421</v>
       </c>
       <c r="F60">
         <v>0</v>
       </c>
       <c r="G60">
-        <v>75315</v>
+        <v>76085</v>
       </c>
       <c r="H60">
         <v>0</v>
@@ -1938,22 +1938,22 @@
         <v>1</v>
       </c>
       <c r="B61">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C61">
-        <v>24778</v>
+        <v>15465</v>
       </c>
       <c r="D61">
         <v>0</v>
       </c>
       <c r="E61">
-        <v>8492</v>
+        <v>4257</v>
       </c>
       <c r="F61">
         <v>0</v>
       </c>
       <c r="G61">
-        <v>16286</v>
+        <v>11208</v>
       </c>
       <c r="H61">
         <v>0</v>
@@ -1964,22 +1964,22 @@
         <v>1</v>
       </c>
       <c r="B62">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C62">
-        <v>137057</v>
+        <v>102132</v>
       </c>
       <c r="D62">
         <v>0</v>
       </c>
       <c r="E62">
-        <v>51757</v>
+        <v>26817</v>
       </c>
       <c r="F62">
         <v>0</v>
       </c>
       <c r="G62">
-        <v>85300</v>
+        <v>75315</v>
       </c>
       <c r="H62">
         <v>0</v>
@@ -1990,22 +1990,22 @@
         <v>1</v>
       </c>
       <c r="B63">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C63">
-        <v>20008</v>
+        <v>24778</v>
       </c>
       <c r="D63">
         <v>0</v>
       </c>
       <c r="E63">
-        <v>5025</v>
+        <v>8492</v>
       </c>
       <c r="F63">
         <v>0</v>
       </c>
       <c r="G63">
-        <v>14983</v>
+        <v>16286</v>
       </c>
       <c r="H63">
         <v>0</v>
@@ -2016,22 +2016,22 @@
         <v>1</v>
       </c>
       <c r="B64">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C64">
-        <v>109424</v>
+        <v>137057</v>
       </c>
       <c r="D64">
         <v>0</v>
       </c>
       <c r="E64">
-        <v>28613</v>
+        <v>51757</v>
       </c>
       <c r="F64">
         <v>0</v>
       </c>
       <c r="G64">
-        <v>80811</v>
+        <v>85300</v>
       </c>
       <c r="H64">
         <v>0</v>
@@ -2042,22 +2042,22 @@
         <v>1</v>
       </c>
       <c r="B65">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C65">
-        <v>11467</v>
+        <v>20008</v>
       </c>
       <c r="D65">
         <v>0</v>
       </c>
       <c r="E65">
-        <v>560</v>
+        <v>5025</v>
       </c>
       <c r="F65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G65">
-        <v>10907</v>
+        <v>14983</v>
       </c>
       <c r="H65">
         <v>0</v>
@@ -2068,22 +2068,22 @@
         <v>1</v>
       </c>
       <c r="B66">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="C66">
-        <v>23067</v>
+        <v>109424</v>
       </c>
       <c r="D66">
         <v>0</v>
       </c>
       <c r="E66">
-        <v>9354</v>
+        <v>28613</v>
       </c>
       <c r="F66">
         <v>0</v>
       </c>
       <c r="G66">
-        <v>13713</v>
+        <v>80811</v>
       </c>
       <c r="H66">
         <v>0</v>
@@ -2094,22 +2094,22 @@
         <v>1</v>
       </c>
       <c r="B67">
-        <v>176</v>
+        <v>85</v>
       </c>
       <c r="C67">
-        <v>26444</v>
+        <v>11467</v>
       </c>
       <c r="D67">
         <v>0</v>
       </c>
       <c r="E67">
-        <v>10749</v>
+        <v>560</v>
       </c>
       <c r="F67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G67">
-        <v>15695</v>
+        <v>10907</v>
       </c>
       <c r="H67">
         <v>0</v>
@@ -2120,24 +2120,128 @@
         <v>1</v>
       </c>
       <c r="B68">
+        <v>96</v>
+      </c>
+      <c r="C68">
+        <v>23067</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>9354</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68">
+        <v>13713</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>1</v>
+      </c>
+      <c r="B69">
+        <v>176</v>
+      </c>
+      <c r="C69">
+        <v>26444</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>10749</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>15695</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>1</v>
+      </c>
+      <c r="B70">
         <v>177</v>
       </c>
-      <c r="C68">
+      <c r="C70">
         <v>8622</v>
       </c>
-      <c r="D68">
-        <v>0</v>
-      </c>
-      <c r="E68">
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
         <v>1419</v>
       </c>
-      <c r="F68">
-        <v>1</v>
-      </c>
-      <c r="G68">
+      <c r="F70">
+        <v>1</v>
+      </c>
+      <c r="G70">
         <v>7203</v>
       </c>
-      <c r="H68">
+      <c r="H70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>1</v>
+      </c>
+      <c r="B71">
+        <v>400</v>
+      </c>
+      <c r="C71">
+        <v>53139880</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>12915617</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>40224264</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>1</v>
+      </c>
+      <c r="B72">
+        <v>451</v>
+      </c>
+      <c r="C72">
+        <v>192733728</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>20750472</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>171983264</v>
+      </c>
+      <c r="H72">
         <v>0</v>
       </c>
     </row>

</xml_diff>